<commit_message>
EPBDS-9041 fix product tests for primitives
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Statistics_product.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Statistics_product.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EIS_Sources\OpenL\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9C949A-03CF-4971-AB71-7131513F6735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="10995"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="13" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2690" uniqueCount="89">
   <si>
     <t>_res_</t>
   </si>
@@ -286,7 +292,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -297,12 +303,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -360,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -379,6 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,7 +452,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -472,9 +485,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -507,6 +537,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -682,50 +729,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:AF105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E67" workbookViewId="0">
-      <selection activeCell="AG89" sqref="AG89"/>
+    <sheetView tabSelected="1" topLeftCell="E40" workbookViewId="0">
+      <selection activeCell="T52" sqref="T52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
-    <col min="2" max="2" width="66.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="79.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.140625" style="2" collapsed="1"/>
-    <col min="11" max="11" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="10.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.140625" style="2"/>
-    <col min="16" max="16" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.109375" style="2" collapsed="1"/>
+    <col min="2" max="2" width="66.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="79.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.109375" style="2" collapsed="1"/>
+    <col min="11" max="11" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="10.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.109375" style="2"/>
+    <col min="16" max="16" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="7.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="6.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="6.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="32" max="32" width="13" style="2" customWidth="1"/>
     <col min="33" max="34" width="13" style="2" customWidth="1" collapsed="1"/>
-    <col min="35" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="35" max="16384" width="9.109375" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>65</v>
       </c>
@@ -766,7 +813,7 @@
       <c r="AD3" s="11"/>
       <c r="AE3" s="11"/>
     </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>63</v>
       </c>
@@ -837,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:31" x14ac:dyDescent="0.3">
       <c r="F5" s="8" t="s">
         <v>41</v>
       </c>
@@ -902,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:31" x14ac:dyDescent="0.3">
       <c r="F6" s="8" t="s">
         <v>42</v>
       </c>
@@ -967,7 +1014,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>75</v>
       </c>
@@ -1038,7 +1085,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>63</v>
       </c>
@@ -1099,7 +1146,7 @@
       </c>
       <c r="AE8" s="5"/>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="D9" s="3"/>
       <c r="F9" s="8" t="s">
@@ -1162,7 +1209,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="D10" s="3"/>
       <c r="F10" s="8" t="s">
@@ -1217,7 +1264,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>77</v>
       </c>
@@ -1288,7 +1335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>63</v>
       </c>
@@ -1309,19 +1356,19 @@
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
     </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>68</v>
       </c>
@@ -1362,7 +1409,7 @@
       <c r="AD16" s="11"/>
       <c r="AE16" s="11"/>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>63</v>
       </c>
@@ -1433,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="F18" s="8" t="s">
@@ -1500,7 +1547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="F19" s="8" t="s">
@@ -1567,7 +1614,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>79</v>
       </c>
@@ -1638,7 +1685,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>63</v>
       </c>
@@ -1699,7 +1746,7 @@
       </c>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
       <c r="D22" s="3"/>
       <c r="F22" s="8" t="s">
@@ -1762,7 +1809,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
       <c r="D23" s="3"/>
       <c r="F23" s="8" t="s">
@@ -1817,7 +1864,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>81</v>
       </c>
@@ -1888,7 +1935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>63</v>
       </c>
@@ -1909,19 +1956,19 @@
       <c r="AD25" s="3"/>
       <c r="AE25" s="3"/>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>70</v>
       </c>
@@ -1962,7 +2009,7 @@
       <c r="AD29" s="11"/>
       <c r="AE29" s="11"/>
     </row>
-    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>63</v>
       </c>
@@ -2033,7 +2080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
       <c r="D31" s="3"/>
       <c r="F31" s="8" t="s">
@@ -2100,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
       <c r="D32" s="3"/>
       <c r="F32" s="8" t="s">
@@ -2167,7 +2214,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>72</v>
       </c>
@@ -2238,7 +2285,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>63</v>
       </c>
@@ -2299,7 +2346,7 @@
       </c>
       <c r="AE34" s="5"/>
     </row>
-    <row r="35" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="8" t="s">
@@ -2362,7 +2409,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B36" s="3"/>
       <c r="D36" s="3"/>
       <c r="F36" s="8" t="s">
@@ -2417,7 +2464,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="37" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>73</v>
       </c>
@@ -2488,7 +2535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>63</v>
       </c>
@@ -2509,7 +2556,7 @@
       <c r="AD38" s="3"/>
       <c r="AE38" s="3"/>
     </row>
-    <row r="39" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B39" s="3"/>
       <c r="D39" s="3"/>
       <c r="L39" s="3"/>
@@ -2521,7 +2568,7 @@
       <c r="AD39" s="3"/>
       <c r="AE39" s="4"/>
     </row>
-    <row r="40" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B40" s="3"/>
       <c r="D40" s="3"/>
       <c r="L40" s="3"/>
@@ -2533,7 +2580,7 @@
       <c r="AD40" s="3"/>
       <c r="AE40" s="4"/>
     </row>
-    <row r="41" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B41" s="3"/>
       <c r="D41" s="3"/>
       <c r="L41" s="4"/>
@@ -2545,7 +2592,7 @@
       <c r="AD41" s="4"/>
       <c r="AE41" s="4"/>
     </row>
-    <row r="42" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>54</v>
       </c>
@@ -2586,7 +2633,7 @@
       <c r="AD42" s="11"/>
       <c r="AE42" s="11"/>
     </row>
-    <row r="43" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>63</v>
       </c>
@@ -2657,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B44" s="3"/>
       <c r="D44" s="3"/>
       <c r="F44" s="8" t="s">
@@ -2724,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B45" s="3"/>
       <c r="D45" s="3"/>
       <c r="F45" s="8" t="s">
@@ -2791,7 +2838,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
         <v>62</v>
       </c>
@@ -2862,7 +2909,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
         <v>63</v>
       </c>
@@ -2907,7 +2954,9 @@
       <c r="V47" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="W47" s="5"/>
+      <c r="W47" s="12">
+        <v>0</v>
+      </c>
       <c r="Y47" s="8" t="s">
         <v>44</v>
       </c>
@@ -2923,7 +2972,7 @@
       </c>
       <c r="AE47" s="5"/>
     </row>
-    <row r="48" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B48" s="3"/>
       <c r="D48" s="3"/>
       <c r="F48" s="8" t="s">
@@ -2986,7 +3035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B49" s="3"/>
       <c r="D49" s="3"/>
       <c r="F49" s="8" t="s">
@@ -3041,7 +3090,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="50" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
         <v>61</v>
       </c>
@@ -3112,7 +3161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>63</v>
       </c>
@@ -3133,19 +3182,19 @@
       <c r="AD51" s="3"/>
       <c r="AE51" s="3"/>
     </row>
-    <row r="52" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>83</v>
       </c>
@@ -3186,7 +3235,7 @@
       <c r="AD55" s="11"/>
       <c r="AE55" s="11"/>
     </row>
-    <row r="56" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
         <v>63</v>
       </c>
@@ -3257,7 +3306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B57" s="3"/>
       <c r="D57" s="3"/>
       <c r="F57" s="8" t="s">
@@ -3324,7 +3373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B58" s="3"/>
       <c r="D58" s="3"/>
       <c r="F58" s="8" t="s">
@@ -3391,7 +3440,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>85</v>
       </c>
@@ -3462,7 +3511,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>63</v>
       </c>
@@ -3523,7 +3572,7 @@
       </c>
       <c r="AE60" s="5"/>
     </row>
-    <row r="61" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B61" s="3"/>
       <c r="D61" s="3"/>
       <c r="F61" s="8" t="s">
@@ -3586,7 +3635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B62" s="3"/>
       <c r="D62" s="3"/>
       <c r="F62" s="8" t="s">
@@ -3641,7 +3690,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="63" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>88</v>
       </c>
@@ -3712,7 +3761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
         <v>63</v>
       </c>
@@ -3733,12 +3782,12 @@
       <c r="AD64" s="3"/>
       <c r="AE64" s="3"/>
     </row>
-    <row r="67" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="V67" s="3"/>
     </row>
-    <row r="68" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="s">
         <v>5</v>
       </c>
@@ -3779,7 +3828,7 @@
       <c r="AD68" s="11"/>
       <c r="AE68" s="11"/>
     </row>
-    <row r="69" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
         <v>63</v>
       </c>
@@ -3850,7 +3899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B70" s="3"/>
       <c r="D70" s="3"/>
       <c r="F70" s="8" t="s">
@@ -3917,7 +3966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B71" s="3"/>
       <c r="D71" s="3"/>
       <c r="F71" s="8" t="s">
@@ -3984,7 +4033,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
         <v>6</v>
       </c>
@@ -4055,7 +4104,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="73" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
         <v>63</v>
       </c>
@@ -4116,7 +4165,7 @@
       </c>
       <c r="AE73" s="5"/>
     </row>
-    <row r="74" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B74" s="3"/>
       <c r="D74" s="3"/>
       <c r="F74" s="8" t="s">
@@ -4179,7 +4228,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B75" s="3"/>
       <c r="D75" s="3"/>
       <c r="F75" s="8" t="s">
@@ -4234,7 +4283,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="76" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B76" s="1" t="s">
         <v>7</v>
       </c>
@@ -4305,7 +4354,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B77" s="1" t="s">
         <v>63</v>
       </c>
@@ -4326,7 +4375,7 @@
       <c r="AD77" s="3"/>
       <c r="AE77" s="3"/>
     </row>
-    <row r="78" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="L78" s="4"/>
@@ -4339,7 +4388,7 @@
       <c r="AD78" s="4"/>
       <c r="AE78" s="4"/>
     </row>
-    <row r="79" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="L79" s="4"/>
@@ -4352,29 +4401,29 @@
       <c r="AD79" s="4"/>
       <c r="AE79" s="4"/>
     </row>
-    <row r="80" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B80" s="3"/>
       <c r="D80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="V80" s="3"/>
     </row>
-    <row r="81" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="V81" s="3"/>
     </row>
-    <row r="82" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="V82" s="3"/>
     </row>
-    <row r="83" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="V83" s="3"/>
     </row>
-    <row r="84" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
         <v>58</v>
       </c>
@@ -4404,7 +4453,7 @@
       <c r="AD84" s="10"/>
       <c r="AE84" s="10"/>
     </row>
-    <row r="85" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B85" s="1" t="s">
         <v>63</v>
       </c>
@@ -4454,7 +4503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K86" s="8" t="s">
         <v>41</v>
       </c>
@@ -4498,7 +4547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K87" s="8" t="s">
         <v>42</v>
       </c>
@@ -4542,7 +4591,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="88" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
         <v>57</v>
       </c>
@@ -4592,7 +4641,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="89" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
         <v>63</v>
       </c>
@@ -4634,7 +4683,7 @@
       </c>
       <c r="AE89" s="5"/>
     </row>
-    <row r="90" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K90" s="8" t="s">
         <v>45</v>
       </c>
@@ -4674,7 +4723,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K91" s="8" t="s">
         <v>46</v>
       </c>
@@ -4706,7 +4755,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="92" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K92" s="5" t="s">
         <v>47</v>
       </c>
@@ -4750,7 +4799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:31" x14ac:dyDescent="0.3">
       <c r="L93" s="3"/>
       <c r="M93" s="3"/>
       <c r="N93" s="3"/>
@@ -4761,7 +4810,7 @@
       <c r="AD93" s="3"/>
       <c r="AE93" s="3"/>
     </row>
-    <row r="96" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
         <v>8</v>
       </c>
@@ -4791,7 +4840,7 @@
       <c r="AD96" s="10"/>
       <c r="AE96" s="10"/>
     </row>
-    <row r="97" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B97" s="1" t="s">
         <v>63</v>
       </c>
@@ -4841,7 +4890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K98" s="8" t="s">
         <v>41</v>
       </c>
@@ -4885,7 +4934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K99" s="8" t="s">
         <v>42</v>
       </c>
@@ -4929,7 +4978,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="100" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B100" s="1" t="s">
         <v>9</v>
       </c>
@@ -4979,7 +5028,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B101" s="1" t="s">
         <v>63</v>
       </c>
@@ -5021,7 +5070,7 @@
       </c>
       <c r="AE101" s="5"/>
     </row>
-    <row r="102" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K102" s="8" t="s">
         <v>45</v>
       </c>
@@ -5061,7 +5110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K103" s="8" t="s">
         <v>46</v>
       </c>
@@ -5093,7 +5142,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="104" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K104" s="5" t="s">
         <v>47</v>
       </c>
@@ -5137,7 +5186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
@@ -5150,26 +5199,11 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="K55:N55"/>
-    <mergeCell ref="P55:S55"/>
-    <mergeCell ref="K68:N68"/>
-    <mergeCell ref="P68:S68"/>
-    <mergeCell ref="P3:S3"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="P16:S16"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="P29:S29"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="K84:N84"/>
-    <mergeCell ref="K96:N96"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="Y96:AA96"/>
+    <mergeCell ref="Y84:AA84"/>
+    <mergeCell ref="U68:W68"/>
+    <mergeCell ref="Y68:AA68"/>
+    <mergeCell ref="AC68:AE68"/>
     <mergeCell ref="AC55:AE55"/>
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="AC16:AE16"/>
@@ -5185,11 +5219,26 @@
     <mergeCell ref="AC29:AE29"/>
     <mergeCell ref="U55:W55"/>
     <mergeCell ref="Y55:AA55"/>
-    <mergeCell ref="Y96:AA96"/>
-    <mergeCell ref="Y84:AA84"/>
-    <mergeCell ref="U68:W68"/>
-    <mergeCell ref="Y68:AA68"/>
-    <mergeCell ref="AC68:AE68"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="K84:N84"/>
+    <mergeCell ref="K96:N96"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="P3:S3"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="P29:S29"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="K55:N55"/>
+    <mergeCell ref="P55:S55"/>
+    <mergeCell ref="K68:N68"/>
+    <mergeCell ref="P68:S68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-7073 refactor product, add tests
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Statistics_product.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Statistics_product.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\openl2\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0AE0D8-F2F0-42C5-909C-C53C9E6E0E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="10995"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="13" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="89">
   <si>
     <t>_res_</t>
   </si>
@@ -211,60 +217,6 @@
     <t>return product(v1, v2);</t>
   </si>
   <si>
-    <t>Method long _byte(byte[] mydata)</t>
-  </si>
-  <si>
-    <t>Method long _byte(byte v1, byte v2)</t>
-  </si>
-  <si>
-    <t>Method long _short(short v1, short v2)</t>
-  </si>
-  <si>
-    <t>Method long _short(short[] mydata)</t>
-  </si>
-  <si>
-    <t>Method long _int(int v1, int v2)</t>
-  </si>
-  <si>
-    <t>Method long _int(int[] mydata)</t>
-  </si>
-  <si>
-    <t>Method Long _Integer(Integer v1, Integer v2)</t>
-  </si>
-  <si>
-    <t>Method Long _Integer(Integer[] mydata)</t>
-  </si>
-  <si>
-    <t>Method LongValue _IntValue(IntValue[] mydata)</t>
-  </si>
-  <si>
-    <t>Method LongValue _IntValue(IntValue v1, IntValue v2)</t>
-  </si>
-  <si>
-    <t>Method Long _Byte(Byte[] mydata)</t>
-  </si>
-  <si>
-    <t>Method Long _Byte(Byte v1, Byte v2)</t>
-  </si>
-  <si>
-    <t>Method LongValue _ByteValue(ByteValue[] mydata)</t>
-  </si>
-  <si>
-    <t>Method LongValue _ByteValue(ByteValue v1, ByteValue v2)</t>
-  </si>
-  <si>
-    <t>Method Long _Short(Short[] mydata)</t>
-  </si>
-  <si>
-    <t>Method Long _Short(Short v1, Short v2)</t>
-  </si>
-  <si>
-    <t>Method LongValue _ShortValue(ShortValue[] mydata)</t>
-  </si>
-  <si>
-    <t>Method LongValue _ShortValue(ShortValue v1, ShortValue v2)</t>
-  </si>
-  <si>
     <t>Method double _float(float[] mydata)</t>
   </si>
   <si>
@@ -283,21 +235,68 @@
     <t>Method DoubleValue _FloatValue(FloatValue[] mydata)</t>
   </si>
   <si>
-    <t>Method short_short(short[] mydata)</t>
-  </si>
-  <si>
-    <t>Method short _short(short[] mydata)</t>
+    <t>Method Double _Byte(Byte v1, Byte v2)</t>
+  </si>
+  <si>
+    <t>Method Double _Byte(Byte[] mydata)</t>
+  </si>
+  <si>
+    <t>Method Double _ByteValue(ByteValue v1, ByteValue v2)</t>
+  </si>
+  <si>
+    <t>Method Double _ByteValue(ByteValue[] mydata)</t>
+  </si>
+  <si>
+    <t>Method Double _byte(byte[] mydata)</t>
+  </si>
+  <si>
+    <t>Method Double _byte(byte v1, byte v2)</t>
+  </si>
+  <si>
+    <t>Method Double _short(short v1, short v2)</t>
+  </si>
+  <si>
+    <t>Method Double _short(short[] mydata)</t>
+  </si>
+  <si>
+    <t>Method Double _Short(Short[] mydata)</t>
+  </si>
+  <si>
+    <t>Method Double _Short(Short v1, Short v2)</t>
+  </si>
+  <si>
+    <t>Method Double _ShortValue(ShortValue v1, ShortValue v2)</t>
+  </si>
+  <si>
+    <t>Method Double _ShortValue(ShortValue[] mydata)</t>
+  </si>
+  <si>
+    <t>Method Double _int(int v1, int v2)</t>
+  </si>
+  <si>
+    <t>Method Double _int(int[] mydata)</t>
+  </si>
+  <si>
+    <t>Method Double _Integer(Integer[] mydata)</t>
+  </si>
+  <si>
+    <t>Method Double _Integer(Integer v1, Integer v2)</t>
+  </si>
+  <si>
+    <t>Method Double _IntValue(IntValue v1, IntValue v2)</t>
+  </si>
+  <si>
+    <t>Method Double _IntValue(IntValue[] mydata)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -365,7 +364,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -388,7 +387,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -404,9 +403,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -444,9 +443,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -479,9 +478,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -514,9 +530,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -689,55 +722,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:AE105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E67" workbookViewId="0">
-      <selection activeCell="AG89" sqref="AG89"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="66.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="79.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="9.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
-    <col min="10" max="10" style="2" width="9.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
-    <col min="12" max="14" bestFit="true" customWidth="true" style="2" width="10.140625" collapsed="true"/>
-    <col min="15" max="15" style="2" width="9.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
-    <col min="17" max="18" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="2" width="18.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="2" width="9.140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="20.42578125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="10.140625" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="2" width="9.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="2" width="10.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" style="2" width="13.0" collapsed="true"/>
-    <col min="33" max="34" customWidth="true" style="2" width="13.0" collapsed="true"/>
-    <col min="35" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.109375" style="2" collapsed="1"/>
+    <col min="2" max="2" width="66.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="79.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="4.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="7.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="6.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.109375" style="2" collapsed="1"/>
+    <col min="11" max="11" width="4.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="14" width="10.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.109375" style="2" collapsed="1"/>
+    <col min="16" max="16" width="4.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="7.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="4.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="9.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="6.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="4.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="4.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="6.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="34" width="13" style="2" customWidth="1" collapsed="1"/>
+    <col min="35" max="16384" width="9.109375" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>10</v>
@@ -773,7 +804,7 @@
       <c r="AD3" s="11"/>
       <c r="AE3" s="11"/>
     </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>63</v>
       </c>
@@ -844,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:31" x14ac:dyDescent="0.3">
       <c r="F5" s="8" t="s">
         <v>41</v>
       </c>
@@ -909,7 +940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:31" x14ac:dyDescent="0.3">
       <c r="F6" s="8" t="s">
         <v>42</v>
       </c>
@@ -974,12 +1005,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>43</v>
@@ -1045,7 +1076,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>63</v>
       </c>
@@ -1090,9 +1121,7 @@
       <c r="V8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="W8" s="5" t="n">
-        <v>0.0</v>
-      </c>
+      <c r="W8" s="5"/>
       <c r="Y8" s="8" t="s">
         <v>44</v>
       </c>
@@ -1108,7 +1137,7 @@
       </c>
       <c r="AE8" s="5"/>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="D9" s="3"/>
       <c r="F9" s="8" t="s">
@@ -1171,7 +1200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="D10" s="3"/>
       <c r="F10" s="8" t="s">
@@ -1226,12 +1255,12 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>47</v>
@@ -1297,7 +1326,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>63</v>
       </c>
@@ -1318,24 +1347,24 @@
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
     </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>13</v>
@@ -1371,7 +1400,7 @@
       <c r="AD16" s="11"/>
       <c r="AE16" s="11"/>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>63</v>
       </c>
@@ -1442,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="F18" s="8" t="s">
@@ -1509,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="F19" s="8" t="s">
@@ -1576,7 +1605,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>79</v>
       </c>
@@ -1647,7 +1676,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>63</v>
       </c>
@@ -1692,9 +1721,7 @@
       <c r="V21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="W21" s="5" t="n">
-        <v>0.0</v>
-      </c>
+      <c r="W21" s="5"/>
       <c r="Y21" s="8" t="s">
         <v>44</v>
       </c>
@@ -1710,7 +1737,7 @@
       </c>
       <c r="AE21" s="5"/>
     </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
       <c r="D22" s="3"/>
       <c r="F22" s="8" t="s">
@@ -1773,7 +1800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
       <c r="D23" s="3"/>
       <c r="F23" s="8" t="s">
@@ -1828,12 +1855,12 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>47</v>
@@ -1899,7 +1926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>63</v>
       </c>
@@ -1920,24 +1947,24 @@
       <c r="AD25" s="3"/>
       <c r="AE25" s="3"/>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>16</v>
@@ -1973,7 +2000,7 @@
       <c r="AD29" s="11"/>
       <c r="AE29" s="11"/>
     </row>
-    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>63</v>
       </c>
@@ -2044,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
       <c r="D31" s="3"/>
       <c r="F31" s="8" t="s">
@@ -2111,7 +2138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
       <c r="D32" s="3"/>
       <c r="F32" s="8" t="s">
@@ -2178,12 +2205,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>43</v>
@@ -2249,7 +2276,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>63</v>
       </c>
@@ -2294,9 +2321,7 @@
       <c r="V34" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="W34" s="5" t="n">
-        <v>0.0</v>
-      </c>
+      <c r="W34" s="5"/>
       <c r="Y34" s="8" t="s">
         <v>44</v>
       </c>
@@ -2312,7 +2337,7 @@
       </c>
       <c r="AE34" s="5"/>
     </row>
-    <row r="35" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="8" t="s">
@@ -2375,7 +2400,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B36" s="3"/>
       <c r="D36" s="3"/>
       <c r="F36" s="8" t="s">
@@ -2430,12 +2455,12 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="37" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>47</v>
@@ -2501,7 +2526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>63</v>
       </c>
@@ -2522,7 +2547,7 @@
       <c r="AD38" s="3"/>
       <c r="AE38" s="3"/>
     </row>
-    <row r="39" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B39" s="3"/>
       <c r="D39" s="3"/>
       <c r="L39" s="3"/>
@@ -2534,7 +2559,7 @@
       <c r="AD39" s="3"/>
       <c r="AE39" s="4"/>
     </row>
-    <row r="40" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B40" s="3"/>
       <c r="D40" s="3"/>
       <c r="L40" s="3"/>
@@ -2546,7 +2571,7 @@
       <c r="AD40" s="3"/>
       <c r="AE40" s="4"/>
     </row>
-    <row r="41" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B41" s="3"/>
       <c r="D41" s="3"/>
       <c r="L41" s="4"/>
@@ -2558,7 +2583,7 @@
       <c r="AD41" s="4"/>
       <c r="AE41" s="4"/>
     </row>
-    <row r="42" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>54</v>
       </c>
@@ -2599,7 +2624,7 @@
       <c r="AD42" s="11"/>
       <c r="AE42" s="11"/>
     </row>
-    <row r="43" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>63</v>
       </c>
@@ -2670,7 +2695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B44" s="3"/>
       <c r="D44" s="3"/>
       <c r="F44" s="8" t="s">
@@ -2737,7 +2762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B45" s="3"/>
       <c r="D45" s="3"/>
       <c r="F45" s="8" t="s">
@@ -2804,7 +2829,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
         <v>62</v>
       </c>
@@ -2875,7 +2900,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
         <v>63</v>
       </c>
@@ -2920,8 +2945,8 @@
       <c r="V47" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="W47" s="5" t="n">
-        <v>0.0</v>
+      <c r="W47" s="5">
+        <v>0</v>
       </c>
       <c r="Y47" s="8" t="s">
         <v>44</v>
@@ -2938,7 +2963,7 @@
       </c>
       <c r="AE47" s="5"/>
     </row>
-    <row r="48" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B48" s="3"/>
       <c r="D48" s="3"/>
       <c r="F48" s="8" t="s">
@@ -3001,7 +3026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B49" s="3"/>
       <c r="D49" s="3"/>
       <c r="F49" s="8" t="s">
@@ -3056,7 +3081,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="50" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
         <v>61</v>
       </c>
@@ -3127,7 +3152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>63</v>
       </c>
@@ -3148,24 +3173,24 @@
       <c r="AD51" s="3"/>
       <c r="AE51" s="3"/>
     </row>
-    <row r="52" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>22</v>
@@ -3201,7 +3226,7 @@
       <c r="AD55" s="11"/>
       <c r="AE55" s="11"/>
     </row>
-    <row r="56" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
         <v>63</v>
       </c>
@@ -3272,7 +3297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B57" s="3"/>
       <c r="D57" s="3"/>
       <c r="F57" s="8" t="s">
@@ -3339,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B58" s="3"/>
       <c r="D58" s="3"/>
       <c r="F58" s="8" t="s">
@@ -3406,12 +3431,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="F59" s="8" t="s">
         <v>43</v>
@@ -3477,7 +3502,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>63</v>
       </c>
@@ -3522,8 +3547,8 @@
       <c r="V60" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="W60" s="5" t="n">
-        <v>0.0</v>
+      <c r="W60" s="5">
+        <v>0</v>
       </c>
       <c r="Y60" s="8" t="s">
         <v>44</v>
@@ -3540,7 +3565,7 @@
       </c>
       <c r="AE60" s="5"/>
     </row>
-    <row r="61" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B61" s="3"/>
       <c r="D61" s="3"/>
       <c r="F61" s="8" t="s">
@@ -3603,7 +3628,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B62" s="3"/>
       <c r="D62" s="3"/>
       <c r="F62" s="8" t="s">
@@ -3658,12 +3683,12 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="63" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>47</v>
@@ -3729,7 +3754,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
         <v>63</v>
       </c>
@@ -3750,12 +3775,12 @@
       <c r="AD64" s="3"/>
       <c r="AE64" s="3"/>
     </row>
-    <row r="67" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="V67" s="3"/>
     </row>
-    <row r="68" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="s">
         <v>5</v>
       </c>
@@ -3796,7 +3821,7 @@
       <c r="AD68" s="11"/>
       <c r="AE68" s="11"/>
     </row>
-    <row r="69" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
         <v>63</v>
       </c>
@@ -3867,7 +3892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B70" s="3"/>
       <c r="D70" s="3"/>
       <c r="F70" s="8" t="s">
@@ -3934,7 +3959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B71" s="3"/>
       <c r="D71" s="3"/>
       <c r="F71" s="8" t="s">
@@ -4001,7 +4026,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
         <v>6</v>
       </c>
@@ -4072,7 +4097,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="73" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
         <v>63</v>
       </c>
@@ -4117,8 +4142,8 @@
       <c r="V73" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="W73" s="5" t="n">
-        <v>0.0</v>
+      <c r="W73" s="5">
+        <v>0</v>
       </c>
       <c r="Y73" s="8" t="s">
         <v>44</v>
@@ -4135,7 +4160,7 @@
       </c>
       <c r="AE73" s="5"/>
     </row>
-    <row r="74" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B74" s="3"/>
       <c r="D74" s="3"/>
       <c r="F74" s="8" t="s">
@@ -4198,7 +4223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B75" s="3"/>
       <c r="D75" s="3"/>
       <c r="F75" s="8" t="s">
@@ -4253,7 +4278,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="76" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B76" s="1" t="s">
         <v>7</v>
       </c>
@@ -4324,7 +4349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B77" s="1" t="s">
         <v>63</v>
       </c>
@@ -4345,7 +4370,7 @@
       <c r="AD77" s="3"/>
       <c r="AE77" s="3"/>
     </row>
-    <row r="78" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="L78" s="4"/>
@@ -4358,7 +4383,7 @@
       <c r="AD78" s="4"/>
       <c r="AE78" s="4"/>
     </row>
-    <row r="79" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="L79" s="4"/>
@@ -4371,29 +4396,29 @@
       <c r="AD79" s="4"/>
       <c r="AE79" s="4"/>
     </row>
-    <row r="80" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B80" s="3"/>
       <c r="D80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="V80" s="3"/>
     </row>
-    <row r="81" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="V81" s="3"/>
     </row>
-    <row r="82" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="V82" s="3"/>
     </row>
-    <row r="83" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="V83" s="3"/>
     </row>
-    <row r="84" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
         <v>58</v>
       </c>
@@ -4423,7 +4448,7 @@
       <c r="AD84" s="10"/>
       <c r="AE84" s="10"/>
     </row>
-    <row r="85" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B85" s="1" t="s">
         <v>63</v>
       </c>
@@ -4473,7 +4498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K86" s="8" t="s">
         <v>41</v>
       </c>
@@ -4517,7 +4542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K87" s="8" t="s">
         <v>42</v>
       </c>
@@ -4561,7 +4586,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="88" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
         <v>57</v>
       </c>
@@ -4611,7 +4636,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="89" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
         <v>63</v>
       </c>
@@ -4653,7 +4678,7 @@
       </c>
       <c r="AE89" s="5"/>
     </row>
-    <row r="90" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K90" s="8" t="s">
         <v>45</v>
       </c>
@@ -4693,7 +4718,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K91" s="8" t="s">
         <v>46</v>
       </c>
@@ -4725,7 +4750,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="92" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K92" s="5" t="s">
         <v>47</v>
       </c>
@@ -4769,7 +4794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:31" x14ac:dyDescent="0.3">
       <c r="L93" s="3"/>
       <c r="M93" s="3"/>
       <c r="N93" s="3"/>
@@ -4780,7 +4805,7 @@
       <c r="AD93" s="3"/>
       <c r="AE93" s="3"/>
     </row>
-    <row r="96" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
         <v>8</v>
       </c>
@@ -4810,7 +4835,7 @@
       <c r="AD96" s="10"/>
       <c r="AE96" s="10"/>
     </row>
-    <row r="97" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B97" s="1" t="s">
         <v>63</v>
       </c>
@@ -4860,7 +4885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K98" s="8" t="s">
         <v>41</v>
       </c>
@@ -4904,7 +4929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K99" s="8" t="s">
         <v>42</v>
       </c>
@@ -4948,7 +4973,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="100" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B100" s="1" t="s">
         <v>9</v>
       </c>
@@ -4998,7 +5023,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B101" s="1" t="s">
         <v>63</v>
       </c>
@@ -5040,7 +5065,7 @@
       </c>
       <c r="AE101" s="5"/>
     </row>
-    <row r="102" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K102" s="8" t="s">
         <v>45</v>
       </c>
@@ -5080,7 +5105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K103" s="8" t="s">
         <v>46</v>
       </c>
@@ -5112,7 +5137,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="104" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:31" x14ac:dyDescent="0.3">
       <c r="K104" s="5" t="s">
         <v>47</v>
       </c>
@@ -5156,7 +5181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:31" x14ac:dyDescent="0.3">
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
@@ -5169,26 +5194,11 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="K55:N55"/>
-    <mergeCell ref="P55:S55"/>
-    <mergeCell ref="K68:N68"/>
-    <mergeCell ref="P68:S68"/>
-    <mergeCell ref="P3:S3"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="P16:S16"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="P29:S29"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="K84:N84"/>
-    <mergeCell ref="K96:N96"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="Y96:AA96"/>
+    <mergeCell ref="Y84:AA84"/>
+    <mergeCell ref="U68:W68"/>
+    <mergeCell ref="Y68:AA68"/>
+    <mergeCell ref="AC68:AE68"/>
     <mergeCell ref="AC55:AE55"/>
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="AC16:AE16"/>
@@ -5204,11 +5214,26 @@
     <mergeCell ref="AC29:AE29"/>
     <mergeCell ref="U55:W55"/>
     <mergeCell ref="Y55:AA55"/>
-    <mergeCell ref="Y96:AA96"/>
-    <mergeCell ref="Y84:AA84"/>
-    <mergeCell ref="U68:W68"/>
-    <mergeCell ref="Y68:AA68"/>
-    <mergeCell ref="AC68:AE68"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="K84:N84"/>
+    <mergeCell ref="K96:N96"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="P3:S3"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="P29:S29"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="K55:N55"/>
+    <mergeCell ref="P55:S55"/>
+    <mergeCell ref="K68:N68"/>
+    <mergeCell ref="P68:S68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>